<commit_message>
concurrent write simulated to verify optimistic concurrency control
</commit_message>
<xml_diff>
--- a/assets/findings.xlsx
+++ b/assets/findings.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t xml:space="preserve">Querying Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loading Time</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">Querying Time (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loading Time (116k Data)</t>
   </si>
   <si>
     <t xml:space="preserve">Source</t>
@@ -52,9 +52,15 @@
     <t xml:space="preserve">0.133570362'</t>
   </si>
   <si>
+    <t xml:space="preserve">Avg</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t xml:space="preserve">Std Dev</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data Size</t>
   </si>
   <si>
@@ -67,45 +73,38 @@
     <t xml:space="preserve">New Size</t>
   </si>
   <si>
-    <t xml:space="preserve">Del Size</t>
+    <t xml:space="preserve">(Del) Size Mb</t>
   </si>
   <si>
     <t xml:space="preserve">1M </t>
   </si>
   <si>
-    <t xml:space="preserve">18.39 Mb</t>
-  </si>
-  <si>
     <t xml:space="preserve">100K</t>
   </si>
   <si>
-    <t xml:space="preserve">1.88 Mb</t>
-  </si>
-  <si>
     <t xml:space="preserve">10K </t>
   </si>
   <si>
-    <t xml:space="preserve">0.18 Mb</t>
-  </si>
-  <si>
     <t xml:space="preserve">1K</t>
   </si>
   <si>
-    <t xml:space="preserve">0.02 Mb</t>
+    <t xml:space="preserve">Avg Change in Size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -127,11 +126,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,37 +190,57 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -405,263 +426,309 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S14" activeCellId="0" sqref="S14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W19" activeCellId="0" sqref="W19:X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>1906435</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="O5" s="1" t="s">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="O5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="O7" s="3" t="s">
+      <c r="L7" s="4"/>
+      <c r="O7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="4" t="n">
+      <c r="P7" s="6" t="n">
         <v>22.089684764</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="7" t="n">
         <v>0.119843644</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5" t="n">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="n">
         <v>0.203098703</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="O8" s="3" t="s">
+      <c r="L8" s="7"/>
+      <c r="O8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="4" t="n">
+      <c r="P8" s="6" t="n">
         <v>9.223035805</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I9" s="5" t="n">
+      <c r="I9" s="7" t="n">
         <v>0.121797024</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5" t="n">
+      <c r="J9" s="7"/>
+      <c r="K9" s="7" t="n">
         <v>0.142536762</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="O9" s="3" t="s">
+      <c r="L9" s="7"/>
+      <c r="O9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="4" t="n">
+      <c r="P9" s="6" t="n">
         <v>8.5139635</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="7" t="n">
         <v>0.198559402</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5" t="n">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7" t="n">
         <v>0.189536395</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5" t="n">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="n">
         <v>0.116369623</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="5" t="n">
+      <c r="I12" s="7" t="n">
         <v>0.121693144</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5" t="n">
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="n">
         <v>0.134754306</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="5" t="n">
+      <c r="I13" s="7" t="n">
         <v>0.16288727</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5" t="n">
+      <c r="J13" s="7"/>
+      <c r="K13" s="7" t="n">
         <v>0.152448842</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="6" t="n">
+      <c r="I14" s="8" t="n">
         <v>0.207689223</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6" t="n">
+      <c r="J14" s="8"/>
+      <c r="K14" s="8" t="n">
         <v>0.125228978</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="6" t="n">
+      <c r="I15" s="8" t="n">
         <v>0.124614096</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6" t="n">
+      <c r="J15" s="8"/>
+      <c r="K15" s="8" t="n">
         <v>0.126862733</v>
       </c>
-      <c r="L15" s="6"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I16" s="5" t="n">
+      <c r="I16" s="7" t="n">
         <v>0.178791003</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5" t="n">
+      <c r="J16" s="7"/>
+      <c r="K16" s="7" t="n">
         <v>0.132328139</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I17" s="5" t="n">
+      <c r="I17" s="7" t="n">
         <v>0.116098403</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5" t="n">
+      <c r="J17" s="7"/>
+      <c r="K17" s="7" t="n">
         <v>0.126504476</v>
       </c>
-      <c r="L17" s="5"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N19" s="0" t="s">
+      <c r="H19" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="I19" s="10" t="n">
+        <f aca="false">AVERAGE(I8:J17)</f>
+        <v>0.150219245444444</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10" t="n">
+        <f aca="false">AVERAGE(K8:K17)</f>
+        <v>0.1449668957</v>
+      </c>
+      <c r="L19" s="10"/>
+      <c r="N19" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O20" s="1" t="s">
+      <c r="H20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="I20" s="10" t="n">
+        <f aca="false">STDEV(I8:J17)</f>
+        <v>0.037048088847071</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10" t="n">
+        <f aca="false">STDEV(K8:L17)</f>
+        <v>0.0289974684079155</v>
+      </c>
+      <c r="L20" s="10"/>
+      <c r="N20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1" t="s">
+      <c r="O21" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="7" t="n">
+      <c r="N22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O22" s="11" t="n">
         <v>2105450</v>
       </c>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7" t="n">
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11" t="n">
         <v>21397959</v>
       </c>
-      <c r="R22" s="7"/>
-      <c r="S22" s="3" t="s">
-        <v>17</v>
+      <c r="R22" s="11"/>
+      <c r="S22" s="5" t="n">
+        <v>18.39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O23" s="7" t="n">
+      <c r="N23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="11" t="n">
         <v>21397959</v>
       </c>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7" t="n">
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11" t="n">
         <v>23373551</v>
       </c>
-      <c r="R23" s="7"/>
-      <c r="S23" s="3" t="s">
-        <v>19</v>
+      <c r="R23" s="11"/>
+      <c r="S23" s="5" t="n">
+        <v>1.88</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N24" s="1" t="s">
+      <c r="N24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O24" s="7" t="n">
+      <c r="O24" s="11" t="n">
         <v>1906435</v>
       </c>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7" t="n">
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11" t="n">
         <v>2105450</v>
       </c>
-      <c r="R24" s="7"/>
-      <c r="S24" s="3" t="s">
+      <c r="R24" s="11"/>
+      <c r="S24" s="5" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N25" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="11" t="n">
+        <v>1881836</v>
+      </c>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11" t="n">
+        <v>1906435</v>
+      </c>
+      <c r="R25" s="11"/>
+      <c r="S25" s="5" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="7" t="n">
-        <v>1881836</v>
-      </c>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7" t="n">
-        <v>1906435</v>
-      </c>
-      <c r="R25" s="7"/>
-      <c r="S25" s="3" t="s">
-        <v>23</v>
+      <c r="R28" s="9"/>
+      <c r="S28" s="10" t="n">
+        <f aca="false">AVERAGE(S22:S25)</f>
+        <v>5.1175</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="R29" s="9"/>
+      <c r="S29" s="12" t="n">
+        <f aca="false">STDEV(S22:S25)</f>
+        <v>8.88827082920707</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="41">
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="I7:J7"/>
@@ -686,6 +753,10 @@
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="K17:L17"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
     <mergeCell ref="O20:S20"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="Q21:R21"/>
@@ -697,6 +768,8 @@
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>